<commit_message>
Fin del proyecto. Integracion realizada.
</commit_message>
<xml_diff>
--- a/backend/data/ventas_2025_06.xlsx
+++ b/backend/data/ventas_2025_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,318 @@
         <v>19500</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S21</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 12</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Motorola G73</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S21</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S21</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Motorola G73</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6500</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 12</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>7000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S21</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Motorola G73</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6500</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>7000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S21</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>iPhone 13</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>18000</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>tarjeta</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>54000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>